<commit_message>
Varios 20 abril 2018
</commit_message>
<xml_diff>
--- a/articulo_dfa/graf_def/Tablas180411_limpio.xlsx
+++ b/articulo_dfa/graf_def/Tablas180411_limpio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVAs" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="77">
   <si>
     <t>Grupo</t>
   </si>
@@ -266,12 +266,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -379,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -408,13 +420,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -426,6 +438,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,7 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+    <sheetView topLeftCell="A117" workbookViewId="0">
       <selection activeCell="S143" sqref="S143"/>
     </sheetView>
   </sheetViews>
@@ -895,7 +910,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -938,7 +953,7 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -979,7 +994,7 @@
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1020,7 +1035,7 @@
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1061,7 +1076,7 @@
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -1104,7 +1119,7 @@
       <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1145,7 +1160,7 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1186,7 +1201,7 @@
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1227,7 +1242,7 @@
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1270,7 +1285,7 @@
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1311,7 +1326,7 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1352,7 +1367,7 @@
       <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1393,7 +1408,7 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="30" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -1436,7 +1451,7 @@
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +1492,7 @@
       <c r="O16" s="6"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1533,7 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1559,7 +1574,7 @@
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1602,7 +1617,7 @@
       <c r="O19" s="11"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1643,7 +1658,7 @@
       <c r="O20" s="6"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1684,7 +1699,7 @@
       <c r="O21" s="6"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1725,7 +1740,7 @@
       <c r="O22" s="7"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -1768,7 +1783,7 @@
       <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1809,7 +1824,7 @@
       <c r="O24" s="6"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1850,7 +1865,7 @@
       <c r="O25" s="6"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1891,7 +1906,7 @@
       <c r="O26" s="7"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="9"/>
@@ -1932,7 +1947,7 @@
       <c r="O27" s="11"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1">
         <v>1</v>
@@ -1971,7 +1986,7 @@
       <c r="O28" s="6"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1">
         <v>1</v>
@@ -2010,7 +2025,7 @@
       <c r="O29" s="6"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
         <v>22</v>
@@ -2049,7 +2064,7 @@
       <c r="O30" s="7"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -2092,7 +2107,7 @@
       <c r="O31" s="11"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
@@ -2133,7 +2148,7 @@
       <c r="O32" s="6"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="1" t="s">
         <v>2</v>
       </c>
@@ -2174,7 +2189,7 @@
       <c r="O33" s="6"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
@@ -2215,7 +2230,7 @@
       <c r="O34" s="7"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="30" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -2258,7 +2273,7 @@
       <c r="O35" s="11"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="1" t="s">
         <v>1</v>
       </c>
@@ -2299,7 +2314,7 @@
       <c r="O36" s="6"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
@@ -2340,7 +2355,7 @@
       <c r="O37" s="6"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="30"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
@@ -2381,7 +2396,7 @@
       <c r="O38" s="7"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -2424,7 +2439,7 @@
       <c r="O39" s="11"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="1" t="s">
         <v>1</v>
       </c>
@@ -2465,7 +2480,7 @@
       <c r="O40" s="6"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="1" t="s">
         <v>2</v>
       </c>
@@ -2506,7 +2521,7 @@
       <c r="O41" s="6"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="30"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -2547,7 +2562,7 @@
       <c r="O42" s="7"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="30" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -2590,7 +2605,7 @@
       <c r="O43" s="11"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="1" t="s">
         <v>1</v>
       </c>
@@ -2631,7 +2646,7 @@
       <c r="O44" s="6"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="1" t="s">
         <v>2</v>
       </c>
@@ -2672,7 +2687,7 @@
       <c r="O45" s="6"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -2713,7 +2728,7 @@
       <c r="O46" s="7"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -2756,7 +2771,7 @@
       <c r="O47" s="11"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="1" t="s">
         <v>1</v>
       </c>
@@ -2797,7 +2812,7 @@
       <c r="O48" s="6"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="1" t="s">
         <v>2</v>
       </c>
@@ -2838,7 +2853,7 @@
       <c r="O49" s="6"/>
     </row>
     <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="30"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="2" t="s">
         <v>8</v>
       </c>
@@ -2879,7 +2894,7 @@
       <c r="O50" s="7"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B51" s="9" t="s">
@@ -2922,7 +2937,7 @@
       <c r="O51" s="11"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -2963,7 +2978,7 @@
       <c r="O52" s="6"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="1" t="s">
         <v>2</v>
       </c>
@@ -3004,7 +3019,7 @@
       <c r="O53" s="6"/>
     </row>
     <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="2" t="s">
         <v>8</v>
       </c>
@@ -3045,7 +3060,7 @@
       <c r="O54" s="7"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B55" s="9" t="s">
@@ -3088,7 +3103,7 @@
       <c r="O55" s="11"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="1" t="s">
         <v>1</v>
       </c>
@@ -3129,7 +3144,7 @@
       <c r="O56" s="6"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="1" t="s">
         <v>2</v>
       </c>
@@ -3170,7 +3185,7 @@
       <c r="O57" s="6"/>
     </row>
     <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="30"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="2" t="s">
         <v>8</v>
       </c>
@@ -3211,7 +3226,7 @@
       <c r="O58" s="7"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="30" t="s">
         <v>27</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -3254,7 +3269,7 @@
       <c r="O59" s="11"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="1" t="s">
         <v>1</v>
       </c>
@@ -3295,7 +3310,7 @@
       <c r="O60" s="6"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="1" t="s">
         <v>2</v>
       </c>
@@ -3336,7 +3351,7 @@
       <c r="O61" s="6"/>
     </row>
     <row r="62" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="30"/>
+      <c r="A62" s="29"/>
       <c r="B62" s="2" t="s">
         <v>8</v>
       </c>
@@ -3377,7 +3392,7 @@
       <c r="O62" s="7"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B63" s="9" t="s">
@@ -3420,7 +3435,7 @@
       <c r="O63" s="11"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="29"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="1" t="s">
         <v>1</v>
       </c>
@@ -3461,7 +3476,7 @@
       <c r="O64" s="6"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="29"/>
+      <c r="A65" s="28"/>
       <c r="B65" s="1" t="s">
         <v>2</v>
       </c>
@@ -3502,7 +3517,7 @@
       <c r="O65" s="6"/>
     </row>
     <row r="66" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="30"/>
+      <c r="A66" s="29"/>
       <c r="B66" s="2" t="s">
         <v>8</v>
       </c>
@@ -3543,7 +3558,7 @@
       <c r="O66" s="7"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
+      <c r="A67" s="30" t="s">
         <v>29</v>
       </c>
       <c r="B67" s="9" t="s">
@@ -3586,7 +3601,7 @@
       <c r="O67" s="11"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
+      <c r="A68" s="28"/>
       <c r="B68" s="1" t="s">
         <v>1</v>
       </c>
@@ -3627,7 +3642,7 @@
       <c r="O68" s="6"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="29"/>
+      <c r="A69" s="28"/>
       <c r="B69" s="1" t="s">
         <v>2</v>
       </c>
@@ -3668,7 +3683,7 @@
       <c r="O69" s="6"/>
     </row>
     <row r="70" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="30"/>
+      <c r="A70" s="29"/>
       <c r="B70" s="2" t="s">
         <v>8</v>
       </c>
@@ -3709,7 +3724,7 @@
       <c r="O70" s="7"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="28" t="s">
+      <c r="A71" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B71" s="9" t="s">
@@ -3752,7 +3767,7 @@
       <c r="O71" s="11"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
+      <c r="A72" s="28"/>
       <c r="B72" s="1" t="s">
         <v>1</v>
       </c>
@@ -3793,7 +3808,7 @@
       <c r="O72" s="6"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="28"/>
       <c r="B73" s="1" t="s">
         <v>2</v>
       </c>
@@ -3834,7 +3849,7 @@
       <c r="O73" s="6"/>
     </row>
     <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="30"/>
+      <c r="A74" s="29"/>
       <c r="B74" s="2" t="s">
         <v>8</v>
       </c>
@@ -3875,7 +3890,7 @@
       <c r="O74" s="7"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="30" t="s">
         <v>31</v>
       </c>
       <c r="B75" s="9" t="s">
@@ -3918,7 +3933,7 @@
       <c r="O75" s="11"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="1" t="s">
         <v>1</v>
       </c>
@@ -3959,7 +3974,7 @@
       <c r="O76" s="6"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="1" t="s">
         <v>2</v>
       </c>
@@ -4000,7 +4015,7 @@
       <c r="O77" s="6"/>
     </row>
     <row r="78" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="30"/>
+      <c r="A78" s="29"/>
       <c r="B78" s="2" t="s">
         <v>8</v>
       </c>
@@ -4041,7 +4056,7 @@
       <c r="O78" s="7"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
+      <c r="A79" s="30" t="s">
         <v>32</v>
       </c>
       <c r="B79" s="9" t="s">
@@ -4084,7 +4099,7 @@
       <c r="O79" s="11"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A80" s="29"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="1" t="s">
         <v>1</v>
       </c>
@@ -4125,7 +4140,7 @@
       <c r="O80" s="6"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A81" s="29"/>
+      <c r="A81" s="28"/>
       <c r="B81" s="1" t="s">
         <v>2</v>
       </c>
@@ -4166,7 +4181,7 @@
       <c r="O81" s="6"/>
     </row>
     <row r="82" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="30"/>
+      <c r="A82" s="29"/>
       <c r="B82" s="2" t="s">
         <v>8</v>
       </c>
@@ -4207,7 +4222,7 @@
       <c r="O82" s="7"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B83" s="9" t="s">
@@ -4250,7 +4265,7 @@
       <c r="O83" s="11"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="28"/>
       <c r="B84" s="1" t="s">
         <v>1</v>
       </c>
@@ -4291,7 +4306,7 @@
       <c r="O84" s="6"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
+      <c r="A85" s="28"/>
       <c r="B85" s="1" t="s">
         <v>2</v>
       </c>
@@ -4332,7 +4347,7 @@
       <c r="O85" s="6"/>
     </row>
     <row r="86" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="30"/>
+      <c r="A86" s="29"/>
       <c r="B86" s="2" t="s">
         <v>8</v>
       </c>
@@ -4373,7 +4388,7 @@
       <c r="O86" s="7"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B87" s="9" t="s">
@@ -4416,7 +4431,7 @@
       <c r="O87" s="11"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="29"/>
+      <c r="A88" s="28"/>
       <c r="B88" s="1" t="s">
         <v>1</v>
       </c>
@@ -4457,7 +4472,7 @@
       <c r="O88" s="6"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
+      <c r="A89" s="28"/>
       <c r="B89" s="1" t="s">
         <v>2</v>
       </c>
@@ -4498,7 +4513,7 @@
       <c r="O89" s="6"/>
     </row>
     <row r="90" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="30"/>
+      <c r="A90" s="29"/>
       <c r="B90" s="2" t="s">
         <v>8</v>
       </c>
@@ -4556,7 +4571,7 @@
       <c r="O91" s="14"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="30" t="s">
         <v>39</v>
       </c>
       <c r="B92" s="9" t="s">
@@ -4599,7 +4614,7 @@
       <c r="O92" s="11"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="28"/>
       <c r="B93" s="1" t="s">
         <v>1</v>
       </c>
@@ -4640,7 +4655,7 @@
       <c r="O93" s="6"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
+      <c r="A94" s="28"/>
       <c r="B94" s="1" t="s">
         <v>2</v>
       </c>
@@ -4681,7 +4696,7 @@
       <c r="O94" s="6"/>
     </row>
     <row r="95" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="30"/>
+      <c r="A95" s="29"/>
       <c r="B95" s="2" t="s">
         <v>8</v>
       </c>
@@ -4722,7 +4737,7 @@
       <c r="O95" s="7"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="s">
+      <c r="A96" s="30" t="s">
         <v>40</v>
       </c>
       <c r="B96" s="9" t="s">
@@ -4765,7 +4780,7 @@
       <c r="O96" s="11"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A97" s="29"/>
+      <c r="A97" s="28"/>
       <c r="B97" s="1" t="s">
         <v>1</v>
       </c>
@@ -4806,7 +4821,7 @@
       <c r="O97" s="6"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A98" s="29"/>
+      <c r="A98" s="28"/>
       <c r="B98" s="1" t="s">
         <v>2</v>
       </c>
@@ -4847,7 +4862,7 @@
       <c r="O98" s="6"/>
     </row>
     <row r="99" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="30"/>
+      <c r="A99" s="29"/>
       <c r="B99" s="2" t="s">
         <v>8</v>
       </c>
@@ -4888,7 +4903,7 @@
       <c r="O99" s="7"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A100" s="28" t="s">
+      <c r="A100" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B100" s="9" t="s">
@@ -4931,7 +4946,7 @@
       <c r="O100" s="11"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A101" s="29"/>
+      <c r="A101" s="28"/>
       <c r="B101" s="1" t="s">
         <v>1</v>
       </c>
@@ -4972,7 +4987,7 @@
       <c r="O101" s="6"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
+      <c r="A102" s="28"/>
       <c r="B102" s="1" t="s">
         <v>2</v>
       </c>
@@ -5013,7 +5028,7 @@
       <c r="O102" s="6"/>
     </row>
     <row r="103" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="30"/>
+      <c r="A103" s="29"/>
       <c r="B103" s="2" t="s">
         <v>8</v>
       </c>
@@ -5054,7 +5069,7 @@
       <c r="O103" s="7"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A104" s="28" t="s">
+      <c r="A104" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B104" s="9" t="s">
@@ -5097,7 +5112,7 @@
       <c r="O104" s="11"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
+      <c r="A105" s="28"/>
       <c r="B105" s="1" t="s">
         <v>1</v>
       </c>
@@ -5138,7 +5153,7 @@
       <c r="O105" s="6"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A106" s="29"/>
+      <c r="A106" s="28"/>
       <c r="B106" s="1" t="s">
         <v>2</v>
       </c>
@@ -5179,7 +5194,7 @@
       <c r="O106" s="6"/>
     </row>
     <row r="107" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="30"/>
+      <c r="A107" s="29"/>
       <c r="B107" s="2" t="s">
         <v>8</v>
       </c>
@@ -5220,7 +5235,7 @@
       <c r="O107" s="7"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="28" t="s">
+      <c r="A108" s="30" t="s">
         <v>43</v>
       </c>
       <c r="B108" s="9" t="s">
@@ -5263,7 +5278,7 @@
       <c r="O108" s="11"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="29"/>
+      <c r="A109" s="28"/>
       <c r="B109" s="1" t="s">
         <v>1</v>
       </c>
@@ -5304,7 +5319,7 @@
       <c r="O109" s="6"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="29"/>
+      <c r="A110" s="28"/>
       <c r="B110" s="1" t="s">
         <v>2</v>
       </c>
@@ -5345,7 +5360,7 @@
       <c r="O110" s="6"/>
     </row>
     <row r="111" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="30"/>
+      <c r="A111" s="29"/>
       <c r="B111" s="2" t="s">
         <v>8</v>
       </c>
@@ -5386,7 +5401,7 @@
       <c r="O111" s="7"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A112" s="28" t="s">
+      <c r="A112" s="30" t="s">
         <v>44</v>
       </c>
       <c r="B112" s="9" t="s">
@@ -5429,7 +5444,7 @@
       <c r="O112" s="11"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A113" s="29"/>
+      <c r="A113" s="28"/>
       <c r="B113" s="1" t="s">
         <v>1</v>
       </c>
@@ -5470,7 +5485,7 @@
       <c r="O113" s="6"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="29"/>
+      <c r="A114" s="28"/>
       <c r="B114" s="1" t="s">
         <v>2</v>
       </c>
@@ -5511,7 +5526,7 @@
       <c r="O114" s="6"/>
     </row>
     <row r="115" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="30"/>
+      <c r="A115" s="29"/>
       <c r="B115" s="2" t="s">
         <v>8</v>
       </c>
@@ -5552,7 +5567,7 @@
       <c r="O115" s="7"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="30" t="s">
         <v>45</v>
       </c>
       <c r="B116" s="9" t="s">
@@ -5595,7 +5610,7 @@
       <c r="O116" s="11"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A117" s="29"/>
+      <c r="A117" s="28"/>
       <c r="B117" s="1" t="s">
         <v>1</v>
       </c>
@@ -5636,7 +5651,7 @@
       <c r="O117" s="6"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A118" s="29"/>
+      <c r="A118" s="28"/>
       <c r="B118" s="1" t="s">
         <v>2</v>
       </c>
@@ -5677,7 +5692,7 @@
       <c r="O118" s="6"/>
     </row>
     <row r="119" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="30"/>
+      <c r="A119" s="29"/>
       <c r="B119" s="2" t="s">
         <v>8</v>
       </c>
@@ -5718,7 +5733,7 @@
       <c r="O119" s="7"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A120" s="28" t="s">
+      <c r="A120" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B120" s="9" t="s">
@@ -5761,7 +5776,7 @@
       <c r="O120" s="11"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A121" s="29"/>
+      <c r="A121" s="28"/>
       <c r="B121" s="1" t="s">
         <v>1</v>
       </c>
@@ -5802,7 +5817,7 @@
       <c r="O121" s="6"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A122" s="29"/>
+      <c r="A122" s="28"/>
       <c r="B122" s="1" t="s">
         <v>2</v>
       </c>
@@ -5843,7 +5858,7 @@
       <c r="O122" s="6"/>
     </row>
     <row r="123" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="30"/>
+      <c r="A123" s="29"/>
       <c r="B123" s="2" t="s">
         <v>8</v>
       </c>
@@ -5884,7 +5899,7 @@
       <c r="O123" s="7"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A124" s="28" t="s">
+      <c r="A124" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B124" s="9" t="s">
@@ -5927,7 +5942,7 @@
       <c r="O124" s="11"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A125" s="29"/>
+      <c r="A125" s="28"/>
       <c r="B125" s="1" t="s">
         <v>1</v>
       </c>
@@ -5968,7 +5983,7 @@
       <c r="O125" s="6"/>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A126" s="29"/>
+      <c r="A126" s="28"/>
       <c r="B126" s="1" t="s">
         <v>2</v>
       </c>
@@ -6009,7 +6024,7 @@
       <c r="O126" s="6"/>
     </row>
     <row r="127" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="30"/>
+      <c r="A127" s="29"/>
       <c r="B127" s="2" t="s">
         <v>8</v>
       </c>
@@ -6050,7 +6065,7 @@
       <c r="O127" s="7"/>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A128" s="29" t="s">
+      <c r="A128" s="28" t="s">
         <v>48</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -6093,7 +6108,7 @@
       <c r="O128" s="6"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A129" s="29"/>
+      <c r="A129" s="28"/>
       <c r="B129" s="1" t="s">
         <v>1</v>
       </c>
@@ -6134,7 +6149,7 @@
       <c r="O129" s="6"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
+      <c r="A130" s="28"/>
       <c r="B130" s="1" t="s">
         <v>2</v>
       </c>
@@ -6175,7 +6190,7 @@
       <c r="O130" s="6"/>
     </row>
     <row r="131" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="30"/>
+      <c r="A131" s="29"/>
       <c r="B131" s="2" t="s">
         <v>8</v>
       </c>
@@ -6216,7 +6231,7 @@
       <c r="O131" s="7"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A132" s="29" t="s">
+      <c r="A132" s="28" t="s">
         <v>49</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -6259,7 +6274,7 @@
       <c r="O132" s="6"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A133" s="29"/>
+      <c r="A133" s="28"/>
       <c r="B133" s="1" t="s">
         <v>1</v>
       </c>
@@ -6300,7 +6315,7 @@
       <c r="O133" s="6"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
+      <c r="A134" s="28"/>
       <c r="B134" s="1" t="s">
         <v>2</v>
       </c>
@@ -6341,7 +6356,7 @@
       <c r="O134" s="6"/>
     </row>
     <row r="135" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="30"/>
+      <c r="A135" s="29"/>
       <c r="B135" s="2" t="s">
         <v>8</v>
       </c>
@@ -6382,7 +6397,7 @@
       <c r="O135" s="7"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A136" s="29" t="s">
+      <c r="A136" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -6425,7 +6440,7 @@
       <c r="O136" s="6"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A137" s="29"/>
+      <c r="A137" s="28"/>
       <c r="B137" s="1" t="s">
         <v>1</v>
       </c>
@@ -6466,7 +6481,7 @@
       <c r="O137" s="6"/>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A138" s="29"/>
+      <c r="A138" s="28"/>
       <c r="B138" s="1" t="s">
         <v>2</v>
       </c>
@@ -6507,7 +6522,7 @@
       <c r="O138" s="6"/>
     </row>
     <row r="139" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="30"/>
+      <c r="A139" s="29"/>
       <c r="B139" s="2" t="s">
         <v>8</v>
       </c>
@@ -6548,7 +6563,7 @@
       <c r="O139" s="7"/>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A140" s="29" t="s">
+      <c r="A140" s="28" t="s">
         <v>51</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -6591,7 +6606,7 @@
       <c r="O140" s="6"/>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A141" s="29"/>
+      <c r="A141" s="28"/>
       <c r="B141" s="1" t="s">
         <v>1</v>
       </c>
@@ -6632,7 +6647,7 @@
       <c r="O141" s="6"/>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A142" s="29"/>
+      <c r="A142" s="28"/>
       <c r="B142" s="1" t="s">
         <v>2</v>
       </c>
@@ -6673,7 +6688,7 @@
       <c r="O142" s="6"/>
     </row>
     <row r="143" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="30"/>
+      <c r="A143" s="29"/>
       <c r="B143" s="2" t="s">
         <v>8</v>
       </c>
@@ -7012,14 +7027,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A136:A139"/>
-    <mergeCell ref="A140:A143"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A132:A135"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
     <mergeCell ref="A108:A111"/>
     <mergeCell ref="A63:A66"/>
     <mergeCell ref="A67:A70"/>
@@ -7032,24 +7057,14 @@
     <mergeCell ref="A96:A99"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="A104:A107"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A136:A139"/>
+    <mergeCell ref="A140:A143"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A132:A135"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G143">
     <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
@@ -8190,10 +8205,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8218,9 +8233,14 @@
     <col min="19" max="19" width="2.140625" customWidth="1"/>
     <col min="20" max="20" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" s="32" t="s">
         <v>35</v>
       </c>
@@ -8246,7 +8266,7 @@
       <c r="T1" s="32"/>
       <c r="U1" s="32"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" s="33" t="s">
         <v>36</v>
       </c>
@@ -8278,7 +8298,7 @@
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
         <v>70</v>
@@ -8329,7 +8349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -8378,7 +8398,7 @@
         <v>3.4536579999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -8427,7 +8447,7 @@
         <v>5.6336879999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -8476,7 +8496,7 @@
         <v>2.8510669999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -8524,8 +8544,17 @@
       <c r="U7" s="3">
         <v>1.9332200000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W7" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA7" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -8573,8 +8602,14 @@
       <c r="U8" s="3">
         <v>1.288155E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z8" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -8622,8 +8657,23 @@
       <c r="U9" s="3">
         <v>6.4237249999999996E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W9" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="X9" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y9" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA9" s="35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -8671,8 +8721,23 @@
       <c r="U10" s="3">
         <v>2.4199410000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W10" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z10" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA10" s="35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -8720,8 +8785,23 @@
       <c r="U11" s="3">
         <v>4.1913909999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W11" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -8769,8 +8849,14 @@
       <c r="U12" s="3">
         <v>7.2846549999999996E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -8819,7 +8905,7 @@
         <v>0.20488429999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -8868,7 +8954,7 @@
         <v>0.62648040000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -8917,7 +9003,7 @@
         <v>9.8071759999999994E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>

</xml_diff>